<commit_message>
test py file added
</commit_message>
<xml_diff>
--- a/resources/world-data-2023.xlsx
+++ b/resources/world-data-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acbcb27dc46e4cd4/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e159d63102df03d/DA Bootcamp/Project 3/Project3Group7/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03590909-58B0-400A-95DE-98D000CBCACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{03590909-58B0-400A-95DE-98D000CBCACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46512211-E101-4218-8255-8EF4D3653365}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="world-data-2023" sheetId="1" r:id="rId1"/>
@@ -2621,7 +2621,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
@@ -3487,20 +3487,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q8" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="17" max="17" width="19.08984375" customWidth="1"/>
-    <col min="28" max="28" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>864</v>
       </c>
@@ -3610,7 +3644,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3717,7 +3751,7 @@
         <v>67.709952999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -3824,7 +3858,7 @@
         <v>20.168330999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -3931,7 +3965,7 @@
         <v>1.659626</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -4008,7 +4042,7 @@
         <v>1.521801</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -4115,7 +4149,7 @@
         <v>17.873887</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -4216,7 +4250,7 @@
         <v>-61.796427999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -4323,7 +4357,7 @@
         <v>-63.616672000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -4430,7 +4464,7 @@
         <v>45.038189000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -4537,7 +4571,7 @@
         <v>133.775136</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -4641,7 +4675,7 @@
         <v>14.550072</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -4748,7 +4782,7 @@
         <v>47.576926999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -4852,7 +4886,7 @@
         <v>-77.396280000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -4956,7 +4990,7 @@
         <v>50.557699999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -5063,7 +5097,7 @@
         <v>90.356330999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -5170,7 +5204,7 @@
         <v>-59.543197999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -5274,7 +5308,7 @@
         <v>27.953389000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -5381,7 +5415,7 @@
         <v>4.4699359999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -5488,7 +5522,7 @@
         <v>-88.497649999999993</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -5595,7 +5629,7 @@
         <v>2.3158340000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -5699,7 +5733,7 @@
         <v>90.433600999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>130</v>
       </c>
@@ -5803,7 +5837,7 @@
         <v>-63.588653000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -5907,7 +5941,7 @@
         <v>17.679075999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>141</v>
       </c>
@@ -6014,7 +6048,7 @@
         <v>24.684866</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>145</v>
       </c>
@@ -6121,7 +6155,7 @@
         <v>-51.925280000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -6219,7 +6253,7 @@
         <v>114.72766900000001</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>155</v>
       </c>
@@ -6326,7 +6360,7 @@
         <v>25.48583</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>160</v>
       </c>
@@ -6433,7 +6467,7 @@
         <v>-1.561593</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>163</v>
       </c>
@@ -6537,7 +6571,7 @@
         <v>29.918886000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -6644,7 +6678,7 @@
         <v>-5.5470800000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>172</v>
       </c>
@@ -6751,7 +6785,7 @@
         <v>-23.041799999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>176</v>
       </c>
@@ -6852,7 +6886,7 @@
         <v>104.99096299999999</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>180</v>
       </c>
@@ -6959,7 +6993,7 @@
         <v>12.354722000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -7066,7 +7100,7 @@
         <v>-106.346771</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -7170,7 +7204,7 @@
         <v>20.939444000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>193</v>
       </c>
@@ -7274,7 +7308,7 @@
         <v>18.732206999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>196</v>
       </c>
@@ -7381,7 +7415,7 @@
         <v>-71.542968999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>200</v>
       </c>
@@ -7488,7 +7522,7 @@
         <v>104.195397</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>206</v>
       </c>
@@ -7595,7 +7629,7 @@
         <v>-74.297332999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>210</v>
       </c>
@@ -7693,7 +7727,7 @@
         <v>43.333300000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>214</v>
       </c>
@@ -7797,7 +7831,7 @@
         <v>15.827659000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>216</v>
       </c>
@@ -7904,7 +7938,7 @@
         <v>-83.753428</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>220</v>
       </c>
@@ -8011,7 +8045,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>225</v>
       </c>
@@ -8103,7 +8137,7 @@
         <v>-77.781166999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>229</v>
       </c>
@@ -8207,7 +8241,7 @@
         <v>33.429859</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>234</v>
       </c>
@@ -8314,7 +8348,7 @@
         <v>15.472962000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -8421,7 +8455,7 @@
         <v>21.758664</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>243</v>
       </c>
@@ -8525,7 +8559,7 @@
         <v>9.5017849999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>248</v>
       </c>
@@ -8626,7 +8660,7 @@
         <v>42.590274999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>252</v>
       </c>
@@ -8718,7 +8752,7 @@
         <v>-61.370975999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>255</v>
       </c>
@@ -8825,7 +8859,7 @@
         <v>-70.162650999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>259</v>
       </c>
@@ -8929,7 +8963,7 @@
         <v>-78.183406000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>263</v>
       </c>
@@ -9033,7 +9067,7 @@
         <v>30.802498</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>268</v>
       </c>
@@ -9137,7 +9171,7 @@
         <v>-88.896529999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>271</v>
       </c>
@@ -9241,7 +9275,7 @@
         <v>10.267894999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>274</v>
       </c>
@@ -9336,7 +9370,7 @@
         <v>39.782333999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>279</v>
       </c>
@@ -9443,7 +9477,7 @@
         <v>25.013607</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>283</v>
       </c>
@@ -9484,7 +9518,7 @@
         <v>31.465865999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>285</v>
       </c>
@@ -9588,7 +9622,7 @@
         <v>40.489673000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>290</v>
       </c>
@@ -9695,7 +9729,7 @@
         <v>178.065032</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>295</v>
       </c>
@@ -9799,7 +9833,7 @@
         <v>25.748151</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>299</v>
       </c>
@@ -9906,7 +9940,7 @@
         <v>2.213749</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>302</v>
       </c>
@@ -10013,7 +10047,7 @@
         <v>11.609444</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>305</v>
       </c>
@@ -10120,7 +10154,7 @@
         <v>-15.310138999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>310</v>
       </c>
@@ -10227,7 +10261,7 @@
         <v>43.356892000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>315</v>
       </c>
@@ -10334,7 +10368,7 @@
         <v>10.451525999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>318</v>
       </c>
@@ -10441,7 +10475,7 @@
         <v>-1.0231939999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>322</v>
       </c>
@@ -10548,7 +10582,7 @@
         <v>21.824311999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>326</v>
       </c>
@@ -10643,7 +10677,7 @@
         <v>-61.679000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>329</v>
       </c>
@@ -10750,7 +10784,7 @@
         <v>-90.230759000000006</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>333</v>
       </c>
@@ -10854,7 +10888,7 @@
         <v>-9.6966450000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>338</v>
       </c>
@@ -10958,7 +10992,7 @@
         <v>-15.180413</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>341</v>
       </c>
@@ -11062,7 +11096,7 @@
         <v>-58.93018</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>345</v>
       </c>
@@ -11166,7 +11200,7 @@
         <v>-72.285214999999994</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>349</v>
       </c>
@@ -11198,7 +11232,7 @@
         <v>12.453389</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>351</v>
       </c>
@@ -11305,7 +11339,7 @@
         <v>-86.241905000000003</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>355</v>
       </c>
@@ -11412,7 +11446,7 @@
         <v>19.503304</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>360</v>
       </c>
@@ -11516,7 +11550,7 @@
         <v>-19.020835000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>365</v>
       </c>
@@ -11623,7 +11657,7 @@
         <v>78.962879999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>371</v>
       </c>
@@ -11730,7 +11764,7 @@
         <v>113.92132700000001</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>377</v>
       </c>
@@ -11837,7 +11871,7 @@
         <v>53.688046</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>382</v>
       </c>
@@ -11944,7 +11978,7 @@
         <v>43.679290999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>386</v>
       </c>
@@ -12048,7 +12082,7 @@
         <v>-8.2438900000000004</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>390</v>
       </c>
@@ -12155,7 +12189,7 @@
         <v>34.851612000000003</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>395</v>
       </c>
@@ -12259,7 +12293,7 @@
         <v>12.56738</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>398</v>
       </c>
@@ -12366,7 +12400,7 @@
         <v>-77.297507999999993</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>403</v>
       </c>
@@ -12470,7 +12504,7 @@
         <v>138.25292400000001</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>406</v>
       </c>
@@ -12577,7 +12611,7 @@
         <v>36.238413999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>410</v>
       </c>
@@ -12684,7 +12718,7 @@
         <v>66.923683999999994</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>415</v>
       </c>
@@ -12791,7 +12825,7 @@
         <v>37.906193000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>420</v>
       </c>
@@ -12880,7 +12914,7 @@
         <v>-157.3768317</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>423</v>
       </c>
@@ -12987,7 +13021,7 @@
         <v>47.481766</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>427</v>
       </c>
@@ -13094,7 +13128,7 @@
         <v>74.766098</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>431</v>
       </c>
@@ -13201,7 +13235,7 @@
         <v>102.495496</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>436</v>
       </c>
@@ -13308,7 +13342,7 @@
         <v>24.603189</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>440</v>
       </c>
@@ -13415,7 +13449,7 @@
         <v>35.862285</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>445</v>
       </c>
@@ -13519,7 +13553,7 @@
         <v>28.233608</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>448</v>
       </c>
@@ -13623,7 +13657,7 @@
         <v>-9.4294989999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>451</v>
       </c>
@@ -13721,7 +13755,7 @@
         <v>17.228331000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>454</v>
       </c>
@@ -13795,7 +13829,7 @@
         <v>9.5209349999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>459</v>
       </c>
@@ -13902,7 +13936,7 @@
         <v>23.881274999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>463</v>
       </c>
@@ -14009,7 +14043,7 @@
         <v>6.1295830000000002</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>467</v>
       </c>
@@ -14116,7 +14150,7 @@
         <v>46.869107</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>471</v>
       </c>
@@ -14223,7 +14257,7 @@
         <v>34.301524999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>475</v>
       </c>
@@ -14330,7 +14364,7 @@
         <v>101.97576599999999</v>
       </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>481</v>
       </c>
@@ -14431,7 +14465,7 @@
         <v>73.220680000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>485</v>
       </c>
@@ -14538,7 +14572,7 @@
         <v>-3.9961660000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>488</v>
       </c>
@@ -14645,7 +14679,7 @@
         <v>14.375416</v>
       </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>493</v>
       </c>
@@ -14734,7 +14768,7 @@
         <v>171.18447800000001</v>
       </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>497</v>
       </c>
@@ -14838,7 +14872,7 @@
         <v>-10.940835</v>
       </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>501</v>
       </c>
@@ -14945,7 +14979,7 @@
         <v>57.552152</v>
       </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>505</v>
       </c>
@@ -15052,7 +15086,7 @@
         <v>-102.552784</v>
       </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>509</v>
       </c>
@@ -15144,7 +15178,7 @@
         <v>150.55081200000001</v>
       </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>512</v>
       </c>
@@ -15251,7 +15285,7 @@
         <v>28.369885</v>
       </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>517</v>
       </c>
@@ -15313,7 +15347,7 @@
         <v>7.4246157999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>520</v>
       </c>
@@ -15420,7 +15454,7 @@
         <v>103.846656</v>
       </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>525</v>
       </c>
@@ -15524,7 +15558,7 @@
         <v>19.374389999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>529</v>
       </c>
@@ -15631,7 +15665,7 @@
         <v>-7.0926200000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>534</v>
       </c>
@@ -15738,7 +15772,7 @@
         <v>35.529561999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>538</v>
       </c>
@@ -15845,7 +15879,7 @@
         <v>95.955973999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>544</v>
       </c>
@@ -15943,7 +15977,7 @@
         <v>18.490410000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>546</v>
       </c>
@@ -15981,7 +16015,7 @@
         <v>166.93150299999999</v>
       </c>
     </row>
-    <row r="123" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>549</v>
       </c>
@@ -16088,7 +16122,7 @@
         <v>84.124008000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>554</v>
       </c>
@@ -16192,7 +16226,7 @@
         <v>5.2912660000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>558</v>
       </c>
@@ -16299,7 +16333,7 @@
         <v>174.88597100000001</v>
       </c>
     </row>
-    <row r="126" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>563</v>
       </c>
@@ -16406,7 +16440,7 @@
         <v>-85.207228999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>567</v>
       </c>
@@ -16513,7 +16547,7 @@
         <v>8.0816660000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>570</v>
       </c>
@@ -16620,7 +16654,7 @@
         <v>8.6752769999999995</v>
       </c>
     </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>575</v>
       </c>
@@ -16709,7 +16743,7 @@
         <v>127.510093</v>
       </c>
     </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>580</v>
       </c>
@@ -16750,7 +16784,7 @@
         <v>21.745274999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>584</v>
       </c>
@@ -16854,7 +16888,7 @@
         <v>8.4689460000000008</v>
       </c>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>589</v>
       </c>
@@ -16961,7 +16995,7 @@
         <v>55.975413000000003</v>
       </c>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>594</v>
       </c>
@@ -17068,7 +17102,7 @@
         <v>69.345116000000004</v>
       </c>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>600</v>
       </c>
@@ -17160,7 +17194,7 @@
         <v>134.58251999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>604</v>
       </c>
@@ -17177,7 +17211,7 @@
         <v>35.233153999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>605</v>
       </c>
@@ -17278,7 +17312,7 @@
         <v>-80.782127000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>608</v>
       </c>
@@ -17385,7 +17419,7 @@
         <v>143.95554999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>613</v>
       </c>
@@ -17492,7 +17526,7 @@
         <v>-58.443832</v>
       </c>
     </row>
-    <row r="139" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>618</v>
       </c>
@@ -17599,7 +17633,7 @@
         <v>-75.015152</v>
       </c>
     </row>
-    <row r="140" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>622</v>
       </c>
@@ -17706,7 +17740,7 @@
         <v>121.774017</v>
       </c>
     </row>
-    <row r="141" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>626</v>
       </c>
@@ -17813,7 +17847,7 @@
         <v>19.145136000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>631</v>
       </c>
@@ -17920,7 +17954,7 @@
         <v>-8.2244539999999997</v>
       </c>
     </row>
-    <row r="143" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>634</v>
       </c>
@@ -18024,7 +18058,7 @@
         <v>51.183883999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>638</v>
       </c>
@@ -18131,7 +18165,7 @@
         <v>24.966760000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>642</v>
       </c>
@@ -18238,7 +18272,7 @@
         <v>105.31875599999999</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>646</v>
       </c>
@@ -18342,7 +18376,7 @@
         <v>29.873888000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>650</v>
       </c>
@@ -18434,7 +18468,7 @@
         <v>-62.782997999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>653</v>
       </c>
@@ -18535,7 +18569,7 @@
         <v>-60.978892999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>656</v>
       </c>
@@ -18636,7 +18670,7 @@
         <v>-61.287227999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>660</v>
       </c>
@@ -18740,7 +18774,7 @@
         <v>-172.10462899999999</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>665</v>
       </c>
@@ -18826,7 +18860,7 @@
         <v>12.457777</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>668</v>
       </c>
@@ -18918,7 +18952,7 @@
         <v>158277</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>671</v>
       </c>
@@ -19025,7 +19059,7 @@
         <v>45.079161999999997</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>675</v>
       </c>
@@ -19132,7 +19166,7 @@
         <v>-14.452362000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>679</v>
       </c>
@@ -19239,7 +19273,7 @@
         <v>21.005859000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>684</v>
       </c>
@@ -19337,7 +19371,7 @@
         <v>55.491976999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>688</v>
       </c>
@@ -19444,7 +19478,7 @@
         <v>-11.779889000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>692</v>
       </c>
@@ -19542,7 +19576,7 @@
         <v>103.819836</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>695</v>
       </c>
@@ -19649,7 +19683,7 @@
         <v>19.699024000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>699</v>
       </c>
@@ -19756,7 +19790,7 @@
         <v>14.995463000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>703</v>
       </c>
@@ -19854,7 +19888,7 @@
         <v>160.156194</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>707</v>
       </c>
@@ -19946,7 +19980,7 @@
         <v>46.199615999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>712</v>
       </c>
@@ -20050,7 +20084,7 @@
         <v>22.937505999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>718</v>
       </c>
@@ -20157,7 +20191,7 @@
         <v>127.76692199999999</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>722</v>
       </c>
@@ -20246,7 +20280,7 @@
         <v>31.3069788</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>726</v>
       </c>
@@ -20353,7 +20387,7 @@
         <v>-3.7492200000000002</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>729</v>
       </c>
@@ -20460,7 +20494,7 @@
         <v>80.771797000000007</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>734</v>
       </c>
@@ -20567,7 +20601,7 @@
         <v>30.217635999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>739</v>
       </c>
@@ -20671,7 +20705,7 @@
         <v>-56.027782999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>743</v>
       </c>
@@ -20775,7 +20809,7 @@
         <v>18.643501000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>748</v>
       </c>
@@ -20879,7 +20913,7 @@
         <v>8.2275120000000008</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>752</v>
       </c>
@@ -20986,7 +21020,7 @@
         <v>38.996814999999998</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>756</v>
       </c>
@@ -21093,7 +21127,7 @@
         <v>71.276093000000003</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>760</v>
       </c>
@@ -21200,7 +21234,7 @@
         <v>34.888821999999998</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>765</v>
       </c>
@@ -21307,7 +21341,7 @@
         <v>100.992541</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>770</v>
       </c>
@@ -21414,7 +21448,7 @@
         <v>125.72753899999999</v>
       </c>
     </row>
-    <row r="177" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>773</v>
       </c>
@@ -21521,7 +21555,7 @@
         <v>0.82478200000000002</v>
       </c>
     </row>
-    <row r="178" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>776</v>
       </c>
@@ -21619,7 +21653,7 @@
         <v>-175.19824199999999</v>
       </c>
     </row>
-    <row r="179" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>781</v>
       </c>
@@ -21726,7 +21760,7 @@
         <v>-61.222503000000003</v>
       </c>
     </row>
-    <row r="180" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>786</v>
       </c>
@@ -21833,7 +21867,7 @@
         <v>9.5374990000000004</v>
       </c>
     </row>
-    <row r="181" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>790</v>
       </c>
@@ -21940,7 +21974,7 @@
         <v>35.243321999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>796</v>
       </c>
@@ -22035,7 +22069,7 @@
         <v>59.556277999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>801</v>
       </c>
@@ -22100,7 +22134,7 @@
         <v>177.64932999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>805</v>
       </c>
@@ -22207,7 +22241,7 @@
         <v>32.290275000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>810</v>
       </c>
@@ -22314,7 +22348,7 @@
         <v>31.165579999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>815</v>
       </c>
@@ -22418,7 +22452,7 @@
         <v>53.847817999999997</v>
       </c>
     </row>
-    <row r="187" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>820</v>
       </c>
@@ -22525,7 +22559,7 @@
         <v>-3.4359730000000002</v>
       </c>
     </row>
-    <row r="188" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>824</v>
       </c>
@@ -22632,7 +22666,7 @@
         <v>-95.712890999999999</v>
       </c>
     </row>
-    <row r="189" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>828</v>
       </c>
@@ -22739,7 +22773,7 @@
         <v>-55.765835000000003</v>
       </c>
     </row>
-    <row r="190" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>832</v>
       </c>
@@ -22840,7 +22874,7 @@
         <v>64.585262</v>
       </c>
     </row>
-    <row r="191" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>837</v>
       </c>
@@ -22944,7 +22978,7 @@
         <v>166.959158</v>
       </c>
     </row>
-    <row r="192" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>841</v>
       </c>
@@ -23048,7 +23082,7 @@
         <v>-66.589730000000003</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>845</v>
       </c>
@@ -23155,7 +23189,7 @@
         <v>108.277199</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>851</v>
       </c>
@@ -23256,7 +23290,7 @@
         <v>48.516387999999999</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>855</v>
       </c>
@@ -23363,7 +23397,7 @@
         <v>27.849332</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>859</v>
       </c>

</xml_diff>